<commit_message>
to run google analytics tools, commited the repository
</commit_message>
<xml_diff>
--- a/project_report.xlsx
+++ b/project_report.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>phase-1</t>
   </si>
@@ -94,6 +94,15 @@
   </si>
   <si>
     <t>Add self evaluation,feedback,report , contact_us,forgot password and signup form</t>
+  </si>
+  <si>
+    <t>phase-4</t>
+  </si>
+  <si>
+    <t>phase-5</t>
+  </si>
+  <si>
+    <t>phase-6</t>
   </si>
 </sst>
 </file>
@@ -116,7 +125,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,13 +134,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
+        <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -148,29 +187,990 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF281A92"/>
+    </mruColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1323975" cy="1297919"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9153525" y="190500"/>
+          <a:ext cx="1323975" cy="1297919"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" cap="none" spc="300">
+            <a:ln w="11430" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="10000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="83000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="200000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="75000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="100000"/>
+                    <a:shade val="50000"/>
+                    <a:satMod val="150000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000"/>
+            </a:gradFill>
+            <a:effectLst>
+              <a:glow rad="45500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="220000"/>
+                  <a:alpha val="35000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" cap="none" spc="300">
+              <a:ln w="11430" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:tint val="10000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:miter lim="800000"/>
+              </a:ln>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="10000">
+                    <a:schemeClr val="accent1">
+                      <a:tint val="83000"/>
+                      <a:shade val="100000"/>
+                      <a:satMod val="200000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="75000">
+                    <a:schemeClr val="accent1">
+                      <a:tint val="100000"/>
+                      <a:shade val="50000"/>
+                      <a:satMod val="150000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000"/>
+              </a:gradFill>
+              <a:effectLst>
+                <a:glow rad="45500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="220000"/>
+                    <a:alpha val="35000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>Compleed</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" cap="none" spc="300">
+              <a:ln w="11430" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:tint val="10000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:miter lim="800000"/>
+              </a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:glow rad="45500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="220000"/>
+                    <a:alpha val="35000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>23-04-2013</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" cap="none" spc="300">
+            <a:ln w="11430" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:glow rad="45500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="220000"/>
+                  <a:alpha val="35000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" cap="none" spc="300">
+              <a:ln w="11430" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:tint val="10000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:miter lim="800000"/>
+              </a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:glow rad="45500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="220000"/>
+                    <a:alpha val="35000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>Added aim and theory</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" cap="none" spc="300">
+            <a:ln w="11430" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="10000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="83000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="200000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="75000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="100000"/>
+                    <a:shade val="50000"/>
+                    <a:satMod val="150000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000"/>
+            </a:gradFill>
+            <a:effectLst>
+              <a:glow rad="45500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="220000"/>
+                  <a:alpha val="35000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1371600" cy="1125693"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10458450" y="1466850"/>
+          <a:ext cx="1371600" cy="1125693"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" cap="none" spc="300">
+            <a:ln w="11430" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="10000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="83000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="200000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="75000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="100000"/>
+                    <a:shade val="50000"/>
+                    <a:satMod val="150000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000"/>
+            </a:gradFill>
+            <a:effectLst>
+              <a:glow rad="45500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="220000"/>
+                  <a:alpha val="35000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" cap="none" spc="300">
+              <a:ln w="11430" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:tint val="10000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:miter lim="800000"/>
+              </a:ln>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="10000">
+                    <a:schemeClr val="accent1">
+                      <a:tint val="83000"/>
+                      <a:shade val="100000"/>
+                      <a:satMod val="200000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="75000">
+                    <a:schemeClr val="accent1">
+                      <a:tint val="100000"/>
+                      <a:shade val="50000"/>
+                      <a:satMod val="150000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000"/>
+              </a:gradFill>
+              <a:effectLst>
+                <a:glow rad="45500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="220000"/>
+                    <a:alpha val="35000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>Compleed</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" cap="none" spc="300">
+              <a:ln w="11430" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:tint val="10000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:miter lim="800000"/>
+              </a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:glow rad="45500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="220000"/>
+                    <a:alpha val="35000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>24-04-2013</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" cap="none" spc="300">
+            <a:ln w="11430" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:glow rad="45500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="220000"/>
+                  <a:alpha val="35000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" cap="none" spc="300">
+              <a:ln w="11430" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:tint val="10000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:miter lim="800000"/>
+              </a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:glow rad="45500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="220000"/>
+                    <a:alpha val="35000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>Added faq</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" cap="none" spc="300">
+            <a:ln w="11430" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="10000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="83000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="200000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="75000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="100000"/>
+                    <a:shade val="50000"/>
+                    <a:satMod val="150000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000"/>
+            </a:gradFill>
+            <a:effectLst>
+              <a:glow rad="45500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="220000"/>
+                  <a:alpha val="35000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1371600" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11839575" y="2590800"/>
+          <a:ext cx="1371600" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" cap="none" spc="300">
+            <a:ln w="11430" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="10000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="83000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="200000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="75000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="100000"/>
+                    <a:shade val="50000"/>
+                    <a:satMod val="150000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000"/>
+            </a:gradFill>
+            <a:effectLst>
+              <a:glow rad="45500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="220000"/>
+                  <a:alpha val="35000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" cap="none" spc="300">
+            <a:ln w="11430" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="10000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="83000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="200000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="75000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="100000"/>
+                    <a:shade val="50000"/>
+                    <a:satMod val="150000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000"/>
+            </a:gradFill>
+            <a:effectLst>
+              <a:glow rad="45500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="220000"/>
+                  <a:alpha val="35000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1371600" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13315950" y="3028950"/>
+          <a:ext cx="1371600" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" cap="none" spc="300">
+            <a:ln w="11430" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="10000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="83000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="200000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="75000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="100000"/>
+                    <a:shade val="50000"/>
+                    <a:satMod val="150000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000"/>
+            </a:gradFill>
+            <a:effectLst>
+              <a:glow rad="45500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="220000"/>
+                  <a:alpha val="35000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" cap="none" spc="300">
+            <a:ln w="11430" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="10000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="83000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="200000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="75000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="100000"/>
+                    <a:shade val="50000"/>
+                    <a:satMod val="150000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000"/>
+            </a:gradFill>
+            <a:effectLst>
+              <a:glow rad="45500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="220000"/>
+                  <a:alpha val="35000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1371600" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14678025" y="3476625"/>
+          <a:ext cx="1371600" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" cap="none" spc="300">
+            <a:ln w="11430" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="10000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="83000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="200000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="75000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="100000"/>
+                    <a:shade val="50000"/>
+                    <a:satMod val="150000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000"/>
+            </a:gradFill>
+            <a:effectLst>
+              <a:glow rad="45500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="220000"/>
+                  <a:alpha val="35000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" cap="none" spc="300">
+            <a:ln w="11430" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="10000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="83000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="200000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="75000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="100000"/>
+                    <a:shade val="50000"/>
+                    <a:satMod val="150000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000"/>
+            </a:gradFill>
+            <a:effectLst>
+              <a:glow rad="45500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="220000"/>
+                  <a:alpha val="35000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1371600" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16078200" y="3876675"/>
+          <a:ext cx="1371600" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" cap="none" spc="300">
+            <a:ln w="11430" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="10000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="83000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="200000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="75000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="100000"/>
+                    <a:shade val="50000"/>
+                    <a:satMod val="150000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000"/>
+            </a:gradFill>
+            <a:effectLst>
+              <a:glow rad="45500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="220000"/>
+                  <a:alpha val="35000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" cap="none" spc="300">
+            <a:ln w="11430" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="10000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="83000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="200000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="75000">
+                  <a:schemeClr val="accent1">
+                    <a:tint val="100000"/>
+                    <a:shade val="50000"/>
+                    <a:satMod val="150000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000"/>
+            </a:gradFill>
+            <a:effectLst>
+              <a:glow rad="45500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="220000"/>
+                  <a:alpha val="35000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -458,52 +1458,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="76" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="75.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" style="7" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="8" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" style="11" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" style="12" customWidth="1"/>
+    <col min="12" max="12" width="21.28515625" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:12" s="10" customFormat="1">
+      <c r="A1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="9" t="s">
         <v>24</v>
       </c>
+      <c r="J1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -513,16 +1526,14 @@
       <c r="C2" s="1">
         <v>41386</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>41387</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -532,101 +1543,79 @@
       <c r="C3" s="1">
         <v>41387</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>41388</v>
       </c>
       <c r="F3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:12" ht="12.75" customHeight="1">
+      <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:12">
       <c r="F5" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:12">
       <c r="F6" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="4"/>
+      <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:12">
       <c r="F7" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:12">
       <c r="F8" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:12">
       <c r="F9" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:12">
       <c r="F10" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:12">
       <c r="F11" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:12">
       <c r="F12" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:12">
       <c r="F13" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:12">
       <c r="F14" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>